<commit_message>
evitar duplicidad de usuarios
</commit_message>
<xml_diff>
--- a/Dataset/dataset_2023-06.xlsx
+++ b/Dataset/dataset_2023-06.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ricardo\Documents\predictive_software\Dataset\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCB24A4-58DE-47D9-B695-A8729D849212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28680" yWindow="1800" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -280,8 +286,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,13 +350,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -388,7 +402,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -422,6 +436,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -456,9 +471,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -631,14 +647,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -646,7 +668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -654,7 +676,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -662,7 +684,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -670,7 +692,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -678,7 +700,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -686,7 +708,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -694,7 +716,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -702,7 +724,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -710,7 +732,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -718,7 +740,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -726,7 +748,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -734,7 +756,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -742,7 +764,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -750,7 +772,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -758,7 +780,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -766,7 +788,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -774,7 +796,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -782,7 +804,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -790,7 +812,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -798,7 +820,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -806,7 +828,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -814,7 +836,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -822,7 +844,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -830,7 +852,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -838,7 +860,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -846,7 +868,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -854,7 +876,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -862,7 +884,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -870,7 +892,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -878,7 +900,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -886,7 +908,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -894,7 +916,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -902,7 +924,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -910,7 +932,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -918,7 +940,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -926,7 +948,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -934,7 +956,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -942,7 +964,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -950,7 +972,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -958,7 +980,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -966,7 +988,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -974,7 +996,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -982,7 +1004,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -990,7 +1012,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -998,7 +1020,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -1006,7 +1028,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1014,7 +1036,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1022,7 +1044,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1030,7 +1052,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -1038,7 +1060,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -1046,7 +1068,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -1054,7 +1076,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -1062,7 +1084,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -1070,7 +1092,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -1078,7 +1100,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -1086,7 +1108,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -1094,7 +1116,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -1102,7 +1124,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -1110,7 +1132,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -1118,7 +1140,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -1126,7 +1148,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -1134,7 +1156,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -1142,7 +1164,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -1150,7 +1172,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -1158,7 +1180,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -1166,7 +1188,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -1174,7 +1196,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -1182,7 +1204,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -1190,7 +1212,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -1198,7 +1220,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -1206,7 +1228,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -1214,7 +1236,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -1222,7 +1244,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -1230,7 +1252,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -1238,7 +1260,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -1246,7 +1268,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -1254,7 +1276,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -1262,7 +1284,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -1270,7 +1292,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -1278,7 +1300,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -1286,7 +1308,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -1294,7 +1316,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>83</v>
       </c>
@@ -1302,7 +1324,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>84</v>
       </c>
@@ -1310,7 +1332,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>85</v>
       </c>
@@ -1318,7 +1340,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>86</v>
       </c>

</xml_diff>